<commit_message>
Added scroll bar to exercise list TrainingView
</commit_message>
<xml_diff>
--- a/Bus, Erweiterungen, Tests.xlsx
+++ b/Bus, Erweiterungen, Tests.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="109">
   <si>
     <t>Kurzbeschreibung</t>
   </si>
@@ -350,9 +350,6 @@
   </si>
   <si>
     <t>Wenn man die Beschreibung einer Einheit immer weiter verlängert, geht der Fokus der Combobox nicht mit</t>
-  </si>
-  <si>
-    <t>Ich kann bei einem aktiven Training nicht in der Liste nach unten scrollen, wenn die Übungen den unteren Rand der Liste überschreiten.</t>
   </si>
 </sst>
 </file>
@@ -787,7 +784,7 @@
   <dimension ref="B2:I38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -868,17 +865,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="2:9" ht="28.55" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
-        <v>109</v>
-      </c>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-      <c r="D6" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="E6" s="2">
-        <v>1</v>
-      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="2"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>

</xml_diff>

<commit_message>
Fixed bug that text is not focused when out of border in editable combobox.
</commit_message>
<xml_diff>
--- a/Bus, Erweiterungen, Tests.xlsx
+++ b/Bus, Erweiterungen, Tests.xlsx
@@ -346,10 +346,10 @@
     <t>... Mit Standardübungssatz im Zufallstraining beobachtet. 2 Runden waren eingestellt. Auch wenn keine Übung angehakt ist, ist das Fragezeichen da. Sollte es aber nicht sein.</t>
   </si>
   <si>
-    <t>Darstellungsfehler</t>
-  </si>
-  <si>
-    <t>Wenn man die Beschreibung einer Einheit immer weiter verlängert, geht der Fokus der Combobox nicht mit</t>
+    <t>Änderungen an voreingestellten Einheiten in den Settings bedürfen eines Tabwechsels</t>
+  </si>
+  <si>
+    <t>User Experience</t>
   </si>
 </sst>
 </file>
@@ -784,7 +784,7 @@
   <dimension ref="B2:I38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -847,17 +847,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:9" ht="28.55" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
-        <v>108</v>
-      </c>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="1"/>
       <c r="C5" s="1"/>
-      <c r="D5" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="E5" s="2">
-        <v>3</v>
-      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="2"/>
       <c r="H5">
         <v>3</v>
       </c>
@@ -866,10 +860,16 @@
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="1"/>
+      <c r="B6" s="1" t="s">
+        <v>107</v>
+      </c>
       <c r="C6" s="1"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="2"/>
+      <c r="D6" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E6" s="2">
+        <v>3</v>
+      </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>

</xml_diff>

<commit_message>
Set some UpdateSourceTriggers to PropertyChanged in ExercisesView and SettingsView to improve user experience.
</commit_message>
<xml_diff>
--- a/Bus, Erweiterungen, Tests.xlsx
+++ b/Bus, Erweiterungen, Tests.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="107">
   <si>
     <t>Kurzbeschreibung</t>
   </si>
@@ -344,12 +344,6 @@
   </si>
   <si>
     <t>... Mit Standardübungssatz im Zufallstraining beobachtet. 2 Runden waren eingestellt. Auch wenn keine Übung angehakt ist, ist das Fragezeichen da. Sollte es aber nicht sein.</t>
-  </si>
-  <si>
-    <t>Änderungen an voreingestellten Einheiten in den Settings bedürfen eines Tabwechsels</t>
-  </si>
-  <si>
-    <t>User Experience</t>
   </si>
 </sst>
 </file>
@@ -784,7 +778,7 @@
   <dimension ref="B2:I38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -860,16 +854,10 @@
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
-        <v>107</v>
-      </c>
+      <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-      <c r="D6" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="E6" s="2">
-        <v>3</v>
-      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="2"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>

</xml_diff>

<commit_message>
Small rework of logic that checks if there are enough exercises available for random training
</commit_message>
<xml_diff>
--- a/Bus, Erweiterungen, Tests.xlsx
+++ b/Bus, Erweiterungen, Tests.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="105">
   <si>
     <t>Kurzbeschreibung</t>
   </si>
@@ -338,12 +338,6 @@
   </si>
   <si>
     <t>Begib dich in Liegestützposition, bei der deine Ellenbogen auf dem Boden aufliegen. Die Hände können sich dabei berühren. Halte diese Position und achte dabei darauf, dass dein Rücken gerade bleibt.</t>
-  </si>
-  <si>
-    <t>Falschmeldung, dass nicht genug  Übungen vorhanden sind, wenn nur Aufwärmübungen oder Dehnübungen aktiv sind</t>
-  </si>
-  <si>
-    <t>... Mit Standardübungssatz im Zufallstraining beobachtet. 2 Runden waren eingestellt. Auch wenn keine Übung angehakt ist, ist das Fragezeichen da. Sollte es aber nicht sein.</t>
   </si>
 </sst>
 </file>
@@ -778,7 +772,7 @@
   <dimension ref="B2:I38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -823,17 +817,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:9" ht="28.55" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>105</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>106</v>
-      </c>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C4" s="1"/>
       <c r="D4" s="3"/>
-      <c r="E4" s="2">
-        <v>3</v>
-      </c>
+      <c r="E4" s="2"/>
       <c r="H4">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
Replaced scores and repeats multiplier in training settings with persisted multiplier in global settings.
</commit_message>
<xml_diff>
--- a/Bus, Erweiterungen, Tests.xlsx
+++ b/Bus, Erweiterungen, Tests.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="245" yWindow="109" windowWidth="14808" windowHeight="8015"/>
+    <workbookView xWindow="245" yWindow="109" windowWidth="14808" windowHeight="8015" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Bugs" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="103">
   <si>
     <t>Kurzbeschreibung</t>
   </si>
@@ -302,12 +302,6 @@
   </si>
   <si>
     <t>Gregor hatte die Idee, dass man auch ein Training über Zeiten gestalten könnte. Idee: Wiederholungen der Übungen werden nicht gewertet. Man kann Pausen und Übungen hinzufügen. Beim Start öffnet sich das Timer-Fenster automatisch und stellt sich immer neu auf die nächste Zeit der Übung bzw. Pause ein, wenn die vorherige abgelaufen ist. Wenn man das Fenster schließt,  wird das Training beendet.</t>
-  </si>
-  <si>
-    <t>Globaler Punktemultiplikator in Settings statt TrainingSettings</t>
-  </si>
-  <si>
-    <t>Durch diese Einstellung kann ich eine feste Anpassung der Wiederholungen und Punkte dauerhaft persistieren. Ein Hinweis kann im Trainingsplanfenster stehen.</t>
   </si>
   <si>
     <t>Stelle dich gerade hin, die Füße stehen nahe beieinander. Beuge dich mit geradem Rücken nach vorn und strecke die Fingerspritzen zu den Zehen.</t>
@@ -771,7 +765,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -1090,7 +1084,7 @@
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="42.8" x14ac:dyDescent="0.25">
@@ -1105,7 +1099,7 @@
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="57.1" x14ac:dyDescent="0.25">
@@ -1120,7 +1114,7 @@
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="42.8" x14ac:dyDescent="0.25">
@@ -1135,7 +1129,7 @@
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="57.1" x14ac:dyDescent="0.25">
@@ -1150,7 +1144,7 @@
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="28.55" x14ac:dyDescent="0.25">
@@ -1165,7 +1159,7 @@
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -1180,7 +1174,7 @@
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
@@ -1298,8 +1292,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -1443,16 +1437,10 @@
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
     </row>
-    <row r="16" spans="2:4" ht="28.55" x14ac:dyDescent="0.25">
-      <c r="B16" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>22</v>
-      </c>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="4"/>
@@ -1636,7 +1624,7 @@
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="28.55" x14ac:dyDescent="0.25">
@@ -2104,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="57.1" x14ac:dyDescent="0.25">
@@ -2138,7 +2126,7 @@
         <v>10</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Bugfixes in for selected category in ExcercisesViewModel
</commit_message>
<xml_diff>
--- a/Bus, Erweiterungen, Tests.xlsx
+++ b/Bus, Erweiterungen, Tests.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="245" yWindow="109" windowWidth="14808" windowHeight="8015" activeTab="1"/>
+    <workbookView xWindow="245" yWindow="109" windowWidth="14808" windowHeight="8015" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Bugs" sheetId="1" r:id="rId1"/>
@@ -17,13 +17,14 @@
     <sheet name="Rücken" sheetId="14" r:id="rId8"/>
     <sheet name="Beine" sheetId="15" r:id="rId9"/>
     <sheet name="Dehnübungen" sheetId="16" r:id="rId10"/>
+    <sheet name="Sheet1" sheetId="17" r:id="rId11"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="205">
   <si>
     <t>Kurzbeschreibung</t>
   </si>
@@ -88,12 +89,6 @@
     <t>Zeittraining einführen</t>
   </si>
   <si>
-    <t xml:space="preserve">Default Übungssatz </t>
-  </si>
-  <si>
-    <t>Fertigstellung</t>
-  </si>
-  <si>
     <t>Überprüfen, ob die Übungen im Übungs-Tab nicht evtl. nach oben sollten</t>
   </si>
   <si>
@@ -109,9 +104,6 @@
     <t>Binding Errors nach Übungen auf Standardeinstellungen zurücksetzen - nachdem man den DateTimePicker genutzt hat</t>
   </si>
   <si>
-    <t>Sie in Du umwandeln</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -295,12 +287,6 @@
     <t>Spagat im Sitzen</t>
   </si>
   <si>
-    <t>Fokustraining Entfernen</t>
-  </si>
-  <si>
-    <t>Das Fokustraining ist im Prinzip sinnlos, man kann auch einfach ein Zirkeltraining mit X Runden und nur einer aktiven Kategorie machen. Vllt sollte ich dann die maximale Rundenanzahl vom Zirkeltraining erhöhen (?)</t>
-  </si>
-  <si>
     <t>Gregor hatte die Idee, dass man auch ein Training über Zeiten gestalten könnte. Idee: Wiederholungen der Übungen werden nicht gewertet. Man kann Pausen und Übungen hinzufügen. Beim Start öffnet sich das Timer-Fenster automatisch und stellt sich immer neu auf die nächste Zeit der Übung bzw. Pause ein, wenn die vorherige abgelaufen ist. Wenn man das Fenster schließt,  wird das Training beendet.</t>
   </si>
   <si>
@@ -332,6 +318,327 @@
   </si>
   <si>
     <t>Begib dich in Liegestützposition, bei der deine Ellenbogen auf dem Boden aufliegen. Die Hände können sich dabei berühren. Halte diese Position und achte dabei darauf, dass dein Rücken gerade bleibt.</t>
+  </si>
+  <si>
+    <t>Sut</t>
+  </si>
+  <si>
+    <t>Testbedingung</t>
+  </si>
+  <si>
+    <t>Erwartetes Ergebnis</t>
+  </si>
+  <si>
+    <t>Check</t>
+  </si>
+  <si>
+    <t>Training Tab</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>Modus: Zirkeltraining</t>
+  </si>
+  <si>
+    <t>Disabled, wenn keine Kategorien angegeben</t>
+  </si>
+  <si>
+    <t>Übungen aller aktiven Kategorien für jede Runde eingeplant, sofern vorhanden</t>
+  </si>
+  <si>
+    <t>Rundenanzahl entspricht den Einstellungen</t>
+  </si>
+  <si>
+    <t>Modus: Zufallstraining</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Übungsanzahl entspricht den Einstellungen</t>
+  </si>
+  <si>
+    <t>Diagramm Y-Achsen Intervalle sind noch seltsam</t>
+  </si>
+  <si>
+    <t>Es werden potentiell aus allen aktiven Kategorien Übungen gewählt</t>
+  </si>
+  <si>
+    <t>Modus: Focustraining</t>
+  </si>
+  <si>
+    <t>Es werden nur Übungen der Kategorie im Fokus eingeplant</t>
+  </si>
+  <si>
+    <t>Modus: Benutzerdefiniertes Training</t>
+  </si>
+  <si>
+    <t>Neue Übung fügt neue Übung ins Training hinzu</t>
+  </si>
+  <si>
+    <t>Neue Überschrift fügt neue Überschrift ins Training hinzu</t>
+  </si>
+  <si>
+    <t>Laden kann genutzt werden, um ein Training zu laden</t>
+  </si>
+  <si>
+    <t>Speichern kann genutzt werden, um ein Training zu speichern.</t>
+  </si>
+  <si>
+    <t>Disabled, wenn keine Übungen im Training</t>
+  </si>
+  <si>
+    <t>In Abhängigkeit vom Modus und aktiven Auf- und Abwärmübungen</t>
+  </si>
+  <si>
+    <t>Zeigt den entsprechenden Text an</t>
+  </si>
+  <si>
+    <t>Aktive Übungskategorien</t>
+  </si>
+  <si>
+    <t>Im Modus Zirkeltraining und Zufallstraining</t>
+  </si>
+  <si>
+    <t>Entspricht den Aktiven Kategorien im Tab Übungen</t>
+  </si>
+  <si>
+    <t>Fragezeichensymbol im Modus</t>
+  </si>
+  <si>
+    <t>Fragezeichensymbol neben Runden</t>
+  </si>
+  <si>
+    <t>Im Modus Zirkeltraining und Zufallstraining und Benutzerdefiniertes Training</t>
+  </si>
+  <si>
+    <t>Speichern ist disabled, wenn keine Übung Im Training ist</t>
+  </si>
+  <si>
+    <t>Nur angezeigt, wenn anhand Wiederholungserlaubnis und Trainingssettings gefordert</t>
+  </si>
+  <si>
+    <t>Übungsliste</t>
+  </si>
+  <si>
+    <t>Stop</t>
+  </si>
+  <si>
+    <t>Gestartetes Focustraining</t>
+  </si>
+  <si>
+    <t>Gestartetes Zufallstraining</t>
+  </si>
+  <si>
+    <t>Gestartetes Benutzerdefiniertes Training</t>
+  </si>
+  <si>
+    <t>Alle Übungen checken beendet das Training, Punkte werden korrekt berechnet angezeigt</t>
+  </si>
+  <si>
+    <t>Gestartetes Zirkeltraining</t>
+  </si>
+  <si>
+    <t>Gestartetes Training, ohne checks</t>
+  </si>
+  <si>
+    <t>Training beendet, ohne Punktegutschrift</t>
+  </si>
+  <si>
+    <t>Training beendet, mit Punktegutschrift</t>
+  </si>
+  <si>
+    <t>Gestartetes Training, mit checks</t>
+  </si>
+  <si>
+    <t>Übung bearbeiten Fenster</t>
+  </si>
+  <si>
+    <t>Alle Eintragungen im Fenster</t>
+  </si>
+  <si>
+    <t>aktualisieren die Übung im Training in Echtzeit</t>
+  </si>
+  <si>
+    <t>i-Symbol</t>
+  </si>
+  <si>
+    <t>Klick öffnet ein Fenster, das die Beschreibung der Übung in Echtzeit ermöglicht</t>
+  </si>
+  <si>
+    <t>Übung Tab</t>
+  </si>
+  <si>
+    <t>Export Button</t>
+  </si>
+  <si>
+    <t>Exportiert den Übungssatz exakt in eine Datei</t>
+  </si>
+  <si>
+    <t>Importiert den Übungssatz exakt aus einer Datei</t>
+  </si>
+  <si>
+    <t>Bezeichnungen der Kategorien</t>
+  </si>
+  <si>
+    <t>Veränderung</t>
+  </si>
+  <si>
+    <t>Aktiv Checkbox der Kategorien</t>
+  </si>
+  <si>
+    <t>Combobox Aufwärmübungen</t>
+  </si>
+  <si>
+    <t>Combobox Abwärmübungen</t>
+  </si>
+  <si>
+    <t>Modus Combobox</t>
+  </si>
+  <si>
+    <t>Wegschalten von Benutzerdefiniertem Training</t>
+  </si>
+  <si>
+    <t>Löscht alle vorhandenen Übungen aus der Übungsliste</t>
+  </si>
+  <si>
+    <t>Passt die Anzahl der Aufwärmübungen für Zirkel- und Zufallstraining an</t>
+  </si>
+  <si>
+    <t>Passt die Anzahl der Abwärmübungen für Zirkel- und Zufallstraining an</t>
+  </si>
+  <si>
+    <t>Speichern Buttons</t>
+  </si>
+  <si>
+    <t>Verwerfen Buttons</t>
+  </si>
+  <si>
+    <t>Veränderung, wenn Übungen der Kategorie unten bearbeitet werden</t>
+  </si>
+  <si>
+    <t>Deaktivierung, wenn Übungen der Kategorie unten bearbeitet werden</t>
+  </si>
+  <si>
+    <t>Verändert die Namen der Kategorien in der Combobox unten, in Training Tab und Traininsplan Tab sowie im Fenster Übung bearbeiten</t>
+  </si>
+  <si>
+    <t>Verändert die verfügbaren Kategorien in der Combobox unten, in Training Tab und Traininsplan Tab sowie im Fenster Übung bearbeiten</t>
+  </si>
+  <si>
+    <t>Name der Übung in Combobox wird angepasst</t>
+  </si>
+  <si>
+    <t>Import Button</t>
+  </si>
+  <si>
+    <t>Import einer Datei, die die in der "Übungen bearbeiten" Combobox ausgewählte Kategorie nicht enthält</t>
+  </si>
+  <si>
+    <t>Kategorie wird in Combobox deselektiert und Übungsliste wird geleert. Hinzufügen Button ist disabled.</t>
+  </si>
+  <si>
+    <t>Zurücksetzen Button</t>
+  </si>
+  <si>
+    <t>Zurücksetzen mit einer in der "Übungen bearbeiten" Combobox ausgewählten Kategorie, die nicht im Standardsatz enthalten ist.</t>
+  </si>
+  <si>
+    <t>Kategorie wird in Combobox umbenannt</t>
+  </si>
+  <si>
+    <t>Import einer Datei, die die in der "Übungen bearbeiten" Combobox ausgewählte Kategorie unter anderem Namen enthält</t>
+  </si>
+  <si>
+    <t>Erste aktive Kategorie wird in der Combobox selektiert und entsprechende Übungen werden angezeigt</t>
+  </si>
+  <si>
+    <t>Mit ungespeicherten Änderungen</t>
+  </si>
+  <si>
+    <t>Setzt ungespeicherte Änderungen zurück</t>
+  </si>
+  <si>
+    <t>Zurücksetzen mit einer in der "Übungen bearbeiten" Combobox ausgewählten Kategorie, die im Standardsatz anders benannt ist.</t>
+  </si>
+  <si>
+    <t>Erste aktive Kategorie wird in der Combobox selektiert und entsprechende Übungen werden angezeigt - falls es in der Datei keine aktiven Kategorien gibt, bleibt die Combobox leer und der Hinzufügenbutton ist disabled</t>
+  </si>
+  <si>
+    <t>Übungen bearbeiten Combobox</t>
+  </si>
+  <si>
+    <t>Enthält die Nammen aller aktiven Übungskategorien</t>
+  </si>
+  <si>
+    <t>Beim Zurücksetzen von Übungen, nachdem ich Zufallstraining ausgewählt habe und fast alle Übungen auf nicht aktiv gesetzt habe</t>
+  </si>
+  <si>
+    <t>Bug siehe Sheet 1</t>
+  </si>
+  <si>
+    <t>Hinzufügen Button</t>
+  </si>
+  <si>
+    <t>Fügt Übung der gewählten Kategorie hinzu</t>
+  </si>
+  <si>
+    <t>Speichert Änderungen separat für Kategorien und Übungen</t>
+  </si>
+  <si>
+    <t>Verwirft Änderungen separat für Kategorien und Übungen</t>
+  </si>
+  <si>
+    <t>Verwirft alle Änderungen und läd den Standardsatz von Übungen</t>
+  </si>
+  <si>
+    <t>Löschen Button einer Übung</t>
+  </si>
+  <si>
+    <t>Ins Training Button einer Übung</t>
+  </si>
+  <si>
+    <t>Löscht die Übung</t>
+  </si>
+  <si>
+    <t>Fügt eine Kopie der Übung dem Training hinzu - beide Kopien beeinflussen sich bei Bearbeitung nicht</t>
+  </si>
+  <si>
+    <t>Übung</t>
+  </si>
+  <si>
+    <t>Einer Auf- oder Abwärmübung</t>
+  </si>
+  <si>
+    <t>Hat keine Punkte</t>
+  </si>
+  <si>
+    <t>Auf- oder Abwärmübung als Kategorie</t>
+  </si>
+  <si>
+    <t>Punkte disabled</t>
+  </si>
+  <si>
+    <t>Einheit Combobox einer Übung</t>
+  </si>
+  <si>
+    <t>Ist gefüllt mit allen Einheiten aus den Einstellungen</t>
+  </si>
+  <si>
+    <t>Aktiv Checkbox einer Übung</t>
+  </si>
+  <si>
+    <t>Deaktiviert</t>
+  </si>
+  <si>
+    <t>Übung wird nicht ins Training eingeplant</t>
+  </si>
+  <si>
+    <t>Beschreibung Button einer Übung</t>
+  </si>
+  <si>
+    <t>Öffnet ein Fenster, dass die Beschreibung der Übung verändert. Schließen speichert die Änderung und enabled den Speichern Button</t>
   </si>
 </sst>
 </file>
@@ -393,7 +700,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -414,12 +721,42 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="16">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -451,14 +788,57 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>44683</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>161726</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="13708925" cy="8313688"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B2:E38" totalsRowShown="0">
   <autoFilter ref="B2:E38"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Kurzbeschreibung" dataDxfId="6"/>
-    <tableColumn id="2" name="Reproduktion" dataDxfId="5"/>
-    <tableColumn id="3" name="Typ" dataDxfId="4"/>
-    <tableColumn id="4" name="Prio [1-3]" dataDxfId="3"/>
+    <tableColumn id="1" name="Kurzbeschreibung" dataDxfId="15"/>
+    <tableColumn id="2" name="Reproduktion" dataDxfId="14"/>
+    <tableColumn id="3" name="Typ" dataDxfId="13"/>
+    <tableColumn id="4" name="Prio [1-3]" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -468,11 +848,50 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="B2:D39" totalsRowShown="0">
   <autoFilter ref="B2:D39"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Kurzbeschreibung" dataDxfId="2"/>
-    <tableColumn id="2" name="Details" dataDxfId="1"/>
-    <tableColumn id="5" name="Typ" dataDxfId="0"/>
+    <tableColumn id="1" name="Kurzbeschreibung" dataDxfId="11"/>
+    <tableColumn id="2" name="Details" dataDxfId="10"/>
+    <tableColumn id="5" name="Typ" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B4:E30" totalsRowShown="0">
+  <autoFilter ref="B4:E30"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Sut" dataDxfId="8"/>
+    <tableColumn id="2" name="Testbedingung" dataDxfId="7"/>
+    <tableColumn id="3" name="Erwartetes Ergebnis" dataDxfId="6"/>
+    <tableColumn id="4" name="Check"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table35" displayName="Table35" ref="B34:E37" totalsRowShown="0">
+  <autoFilter ref="B34:E37"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Sut" dataDxfId="5"/>
+    <tableColumn id="2" name="Testbedingung" dataDxfId="4"/>
+    <tableColumn id="3" name="Erwartetes Ergebnis" dataDxfId="3"/>
+    <tableColumn id="4" name="Check"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table36" displayName="Table36" ref="B41:E65" totalsRowShown="0">
+  <autoFilter ref="B41:E65"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Sut" dataDxfId="2"/>
+    <tableColumn id="2" name="Testbedingung" dataDxfId="1"/>
+    <tableColumn id="3" name="Erwartetes Ergebnis" dataDxfId="0"/>
+    <tableColumn id="4" name="Check"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -766,7 +1185,7 @@
   <dimension ref="B2:I38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -794,7 +1213,7 @@
     </row>
     <row r="3" spans="2:9" ht="28.55" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="3"/>
@@ -812,6 +1231,9 @@
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>183</v>
+      </c>
       <c r="C4" s="1"/>
       <c r="D4" s="3"/>
       <c r="E4" s="2"/>
@@ -1057,124 +1479,124 @@
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>29</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="3" spans="2:6" ht="28.55" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C3" s="1">
         <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="42.8" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C4" s="1">
         <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="57.1" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C5" s="1">
         <v>3</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="42.8" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C6" s="1">
         <v>3</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="57.1" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C7" s="1">
         <v>3</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="28.55" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C8" s="1">
         <v>3</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="71.349999999999994" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C9" s="1">
         <v>3</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
@@ -1285,6 +1707,27 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B48"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q56" sqref="Q56"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>182</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1292,8 +1735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:D16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -1363,20 +1806,16 @@
         <v>20</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="4" t="s">
-        <v>21</v>
-      </c>
+      <c r="B8" s="4"/>
       <c r="C8" s="4"/>
-      <c r="D8" s="4" t="s">
-        <v>22</v>
-      </c>
+      <c r="D8" s="4"/>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="4"/>
@@ -1385,19 +1824,19 @@
     </row>
     <row r="10" spans="2:4" ht="28.55" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="28.55" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>13</v>
@@ -1412,25 +1851,17 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:4" ht="28.55" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
-        <v>28</v>
+        <v>111</v>
       </c>
       <c r="C13" s="4"/>
-      <c r="D13" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" ht="28.55" x14ac:dyDescent="0.25">
-      <c r="B14" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>22</v>
-      </c>
+      <c r="D13" s="4"/>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="4"/>
@@ -1570,13 +2001,664 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B2:E65"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C78" sqref="C78"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="3" width="31.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="29.875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="8" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" ht="42.8" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="D6" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="D7" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E7" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="C8" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E8" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="D9" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" ht="42.8" x14ac:dyDescent="0.25">
+      <c r="D10" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E10" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="C11" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E11" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="D12" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E12" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="D13" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E13" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="D14" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E14" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="C15" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E15" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="D16" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E16" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="D17" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E17" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="D18" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E18" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="D19" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E19" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="D20" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E20" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E21" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E22" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="B23" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E23" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" ht="42.8" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E24" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" ht="42.8" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E25" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C26" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E26" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C27" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E27" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="C28" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E28" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="B29" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E29" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="C30" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E30" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="8" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B34" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E34" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="B35" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E35" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="B36" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="E36" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" ht="42.8" x14ac:dyDescent="0.25">
+      <c r="B37" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E37" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B39" s="8" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B41" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E41" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="B42" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E42" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="C43" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E43" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="B44" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E44" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" ht="99.85" x14ac:dyDescent="0.25">
+      <c r="C45" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="E45" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" ht="57.1" x14ac:dyDescent="0.25">
+      <c r="C46" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E46" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" ht="71.349999999999994" x14ac:dyDescent="0.25">
+      <c r="B47" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="E47" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="C48" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="E48" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" ht="71.349999999999994" x14ac:dyDescent="0.25">
+      <c r="B49" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="E49" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" ht="57.1" x14ac:dyDescent="0.25">
+      <c r="C50" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E50" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" ht="42.8" x14ac:dyDescent="0.25">
+      <c r="B51" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E51" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" ht="42.8" x14ac:dyDescent="0.25">
+      <c r="B52" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E52" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="B53" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="E53" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="B54" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="E54" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="B55" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E55" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="B56" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E56" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B57" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="E57" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B58" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E58" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5" ht="57.1" x14ac:dyDescent="0.25">
+      <c r="B59" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="E59" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="B60" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="E60" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="61" spans="2:5" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="B61" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="E61" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="62" spans="2:5" ht="71.349999999999994" x14ac:dyDescent="0.25">
+      <c r="B62" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="E62" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="63" spans="2:5" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="B63" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E63" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="64" spans="2:5" ht="57.1" x14ac:dyDescent="0.25">
+      <c r="C64" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="E64" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="65" spans="3:5" ht="57.1" x14ac:dyDescent="0.25">
+      <c r="C65" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E65" t="s">
+        <v>109</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="3">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -1597,79 +2679,79 @@
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>29</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="3" spans="2:6" ht="57.1" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C3" s="1">
         <v>60</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="28.55" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C4" s="1">
         <v>60</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="42.8" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C5" s="1">
         <v>60</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="42.8" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C6" s="1">
         <v>15</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
@@ -1814,87 +2896,87 @@
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>29</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="3" spans="2:6" ht="42.8" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C3" s="1">
         <v>20</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E3" s="1">
         <v>10</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="42.8" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C4" s="1">
         <v>20</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E4" s="1">
         <v>10</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="114.15" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C5" s="1">
         <v>15</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E5" s="1">
         <v>10</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="85.6" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C6" s="1">
         <v>20</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E6" s="1">
         <v>10</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
@@ -2046,87 +3128,87 @@
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>29</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="3" spans="2:6" ht="71.349999999999994" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C3" s="1">
         <v>30</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E3" s="1">
         <v>10</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="42.8" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C4" s="1">
         <v>90</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E4" s="1">
         <v>10</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="57.1" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C5" s="1">
         <v>20</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E5" s="1">
         <v>10</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="114.15" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C6" s="1">
         <v>20</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E6" s="1">
         <v>10</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
@@ -2275,87 +3357,87 @@
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>29</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="3" spans="2:6" ht="99.85" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C3" s="1">
         <v>10</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E3" s="1">
         <v>10</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="71.349999999999994" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C4" s="1">
         <v>25</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E4" s="1">
         <v>10</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="57.1" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C5" s="1">
         <v>30</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E5" s="1">
         <v>10</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="57.1" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C6" s="1">
         <v>25</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E6" s="1">
         <v>10</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
@@ -2507,87 +3589,87 @@
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>29</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="3" spans="2:6" ht="71.349999999999994" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C3">
         <v>4</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E3" s="1">
         <v>10</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="28.55" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C4" s="1">
         <v>20</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E4" s="1">
         <v>10</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="99.85" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C5" s="1">
         <v>20</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E5" s="1">
         <v>10</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="114.15" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C6" s="1">
         <v>20</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E6" s="1">
         <v>10</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
@@ -2739,87 +3821,87 @@
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>29</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="3" spans="2:6" ht="71.349999999999994" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C3" s="1">
         <v>15</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E3" s="1">
         <v>10</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="42.8" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C4" s="1">
         <v>8</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E4" s="1">
         <v>10</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="71.349999999999994" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C5" s="1">
         <v>50</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E5" s="1">
         <v>10</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="71.349999999999994" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C6" s="1">
         <v>15</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E6" s="1">
         <v>10</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Refactored Settings to save changes instantly; moved Import and Export buttons down in ExerciseView; fixed bug in ExerciseAvailabilityChecker
</commit_message>
<xml_diff>
--- a/Bus, Erweiterungen, Tests.xlsx
+++ b/Bus, Erweiterungen, Tests.xlsx
@@ -19,12 +19,12 @@
     <sheet name="Dehnübungen" sheetId="16" r:id="rId10"/>
     <sheet name="Sheet1" sheetId="17" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="276">
   <si>
     <t>Kurzbeschreibung</t>
   </si>
@@ -639,13 +639,229 @@
   </si>
   <si>
     <t>Öffnet ein Fenster, dass die Beschreibung der Übung verändert. Schließen speichert die Änderung und enabled den Speichern Button</t>
+  </si>
+  <si>
+    <t>Trainingsplan Tab - Reiter "Einsehen"</t>
+  </si>
+  <si>
+    <t>Punkte aktueller Monat</t>
+  </si>
+  <si>
+    <t>Monat wird korrekt angezeigt.</t>
+  </si>
+  <si>
+    <t>Balken wird gefüllt
+Gesamtpunkte werden aktualisiert
+Übersicht wird aktualisiert
+Kopie in Detailansicht wird aktualisiert</t>
+  </si>
+  <si>
+    <t>Punkte Gesamtzeitraum</t>
+  </si>
+  <si>
+    <t>Kategorie Gesamt wird ausgewählt, deaktivierte Kategorie ist weder in Übersicht noch in Details vorhanden</t>
+  </si>
+  <si>
+    <t>Name in Combobox und Detailansicht aktualisiert</t>
+  </si>
+  <si>
+    <t>Kein Punkteziel für aktuellen Monat</t>
+  </si>
+  <si>
+    <t>Mit Punkteziel für aktuellen Monat</t>
+  </si>
+  <si>
+    <t>Anzeige "von [Gesamtpunktzahl]"</t>
+  </si>
+  <si>
+    <t>keine Anzeige "von [Gesamtpunktzahl]"</t>
+  </si>
+  <si>
+    <t>Vorher gespeicherte Punkte werden wiederhergestellt</t>
+  </si>
+  <si>
+    <t>Manuelle Änderung von Punkten, Zeitbasierter Trainingsplan</t>
+  </si>
+  <si>
+    <t>Automatisches Hinzufügen von Punkten nach Trainingsabschluss, Zeitbasierter Trainingsplan</t>
+  </si>
+  <si>
+    <t>In Combobox gewählte Kategorie wird deaktiviert, Zeitbasierter Trainingsplan</t>
+  </si>
+  <si>
+    <t>In Combobox gewählte Kategorie wird reaktiviert, Zeitbasierter Trainingsplan</t>
+  </si>
+  <si>
+    <t>In Combobox gewählte Kategorie wird umbenannt, Zeitbasierter Trainingsplan</t>
+  </si>
+  <si>
+    <t>Trainingsplan Tab - Reiter "Bearbeiten"</t>
+  </si>
+  <si>
+    <t>Fortlaufendes Training</t>
+  </si>
+  <si>
+    <t>Punktetextboxen</t>
+  </si>
+  <si>
+    <t>alle edtitierbar, Namen und Vorhandensein der Kategorien entspricht den Einstellungen im Übungen-Tab</t>
+  </si>
+  <si>
+    <t>Speichern Button</t>
+  </si>
+  <si>
+    <t>Speichert Punktevorgaben für jeden Monat korrekt ab.</t>
+  </si>
+  <si>
+    <t>Verwerfen Button</t>
+  </si>
+  <si>
+    <t>Verwirft ungespeicherte Änderungen</t>
+  </si>
+  <si>
+    <t>Trainingsplan Löschen Button</t>
+  </si>
+  <si>
+    <t>Trainingpunkte Löschen Button</t>
+  </si>
+  <si>
+    <t>Reset der gespeicherten Punktevorgaben</t>
+  </si>
+  <si>
+    <t>Reset der gespeicherten Punkte ohne Reset der Punktevorgaben</t>
+  </si>
+  <si>
+    <t>Zeitbasiertes Training</t>
+  </si>
+  <si>
+    <t>Dauer Combobox</t>
+  </si>
+  <si>
+    <t>Änderung fügt neue Punktetextboxen hinzu</t>
+  </si>
+  <si>
+    <t>Änderung Ändert Überschriften der Punktetextboxen</t>
+  </si>
+  <si>
+    <t>Startdatum Combobox</t>
+  </si>
+  <si>
+    <t>Punkte stimmen mit denen des aktuellen Monats überein,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Zeitbasierter Trainingsplan, Details Ansicht</t>
+  </si>
+  <si>
+    <t>Aktivierung entsprechdend der Radiobuttons für Verteilung der Punkte</t>
+  </si>
+  <si>
+    <t>Zeitbasiertes Training, Gesamtpunkte automatisch berechnen</t>
+  </si>
+  <si>
+    <t>Automatische Bererchnung ist korrekt</t>
+  </si>
+  <si>
+    <t>Zeitbasiertes Training, Gesamtpunkte gleichmäßig verteilen</t>
+  </si>
+  <si>
+    <t>Verteilung ist korrekt</t>
+  </si>
+  <si>
+    <t>Einstellungen Tab</t>
+  </si>
+  <si>
+    <t>Entfernen Button</t>
+  </si>
+  <si>
+    <t>keine Texteingabe einer Einheit</t>
+  </si>
+  <si>
+    <t>nach Texteingabe einer Einheit</t>
+  </si>
+  <si>
+    <t>Disabled</t>
+  </si>
+  <si>
+    <t>Fügt den Text der Tabelle hinzu und löscht die Textbox</t>
+  </si>
+  <si>
+    <t>ohne Selektierung einer Einheit</t>
+  </si>
+  <si>
+    <t>mit Selektierung einer Einheit</t>
+  </si>
+  <si>
+    <t>Löscht die Einheit</t>
+  </si>
+  <si>
+    <t>direkt nach Hinzufügen</t>
+  </si>
+  <si>
+    <t>Die neue Einheit ist im Übungstab und im Fenster zum Übung bearbeiten vorhanden</t>
+  </si>
+  <si>
+    <t>Die neue Einheit ist nicht mehr im Übungstab und im Fenster zum Übung bearbeiten vorhanden</t>
+  </si>
+  <si>
+    <t>Multiplikatoren</t>
+  </si>
+  <si>
+    <t>Funktionieren</t>
+  </si>
+  <si>
+    <t>Änderung Ändert Löscht erreichte Punkte nach Benutzerbestätigung</t>
+  </si>
+  <si>
+    <t>Typ Combobox</t>
+  </si>
+  <si>
+    <t>Wiederholungen erlauben Combobox</t>
+  </si>
+  <si>
+    <t>Hinweis Text korrekt</t>
+  </si>
+  <si>
+    <t>Wiederholung in automatischen Trainings entspricht der Einstellung, Hinweis wird im Training Tab angezeigt, wenn nicht genug Übungen vorhanden sind.</t>
+  </si>
+  <si>
+    <t>Resettet die Einstellungen</t>
+  </si>
+  <si>
+    <t>Allgemeines</t>
+  </si>
+  <si>
+    <t>Anzeigetexte</t>
+  </si>
+  <si>
+    <t>Texte in eingeblendeten Hinweisen</t>
+  </si>
+  <si>
+    <t>Verständlich und Fehlerfrei</t>
+  </si>
+  <si>
+    <t>Start ohne Save Datei</t>
+  </si>
+  <si>
+    <t>direkt nach Entfernen</t>
+  </si>
+  <si>
+    <t>Einheiten-Liste, Multiplikatoren und Wiederholungserlaubnis</t>
+  </si>
+  <si>
+    <t>direkt nach Änderung</t>
+  </si>
+  <si>
+    <t>Änderung nach Neustart noch vorhanden</t>
+  </si>
+  <si>
+    <t>Nutzt Defaults für alle gespeicherten Daten und legt eine neue Save Datei an.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -669,16 +885,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -695,12 +931,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -724,12 +989,386 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="38">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <right style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -835,10 +1474,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B2:E38" totalsRowShown="0">
   <autoFilter ref="B2:E38"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Kurzbeschreibung" dataDxfId="15"/>
-    <tableColumn id="2" name="Reproduktion" dataDxfId="14"/>
-    <tableColumn id="3" name="Typ" dataDxfId="13"/>
-    <tableColumn id="4" name="Prio [1-3]" dataDxfId="12"/>
+    <tableColumn id="1" name="Kurzbeschreibung" dataDxfId="37"/>
+    <tableColumn id="2" name="Reproduktion" dataDxfId="36"/>
+    <tableColumn id="3" name="Typ" dataDxfId="35"/>
+    <tableColumn id="4" name="Prio [1-3]" dataDxfId="34"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -848,9 +1487,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="B2:D39" totalsRowShown="0">
   <autoFilter ref="B2:D39"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Kurzbeschreibung" dataDxfId="11"/>
-    <tableColumn id="2" name="Details" dataDxfId="10"/>
-    <tableColumn id="5" name="Typ" dataDxfId="9"/>
+    <tableColumn id="1" name="Kurzbeschreibung" dataDxfId="33"/>
+    <tableColumn id="2" name="Details" dataDxfId="32"/>
+    <tableColumn id="5" name="Typ" dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -860,9 +1499,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B4:E30" totalsRowShown="0">
   <autoFilter ref="B4:E30"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Sut" dataDxfId="8"/>
-    <tableColumn id="2" name="Testbedingung" dataDxfId="7"/>
-    <tableColumn id="3" name="Erwartetes Ergebnis" dataDxfId="6"/>
+    <tableColumn id="1" name="Sut" dataDxfId="30"/>
+    <tableColumn id="2" name="Testbedingung" dataDxfId="29"/>
+    <tableColumn id="3" name="Erwartetes Ergebnis" dataDxfId="28"/>
     <tableColumn id="4" name="Check"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -873,6 +1512,58 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table35" displayName="Table35" ref="B34:E37" totalsRowShown="0">
   <autoFilter ref="B34:E37"/>
   <tableColumns count="4">
+    <tableColumn id="1" name="Sut" dataDxfId="27"/>
+    <tableColumn id="2" name="Testbedingung" dataDxfId="26"/>
+    <tableColumn id="3" name="Erwartetes Ergebnis" dataDxfId="25"/>
+    <tableColumn id="4" name="Check"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table36" displayName="Table36" ref="B41:E65" totalsRowShown="0">
+  <autoFilter ref="B41:E65"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Sut" dataDxfId="24"/>
+    <tableColumn id="2" name="Testbedingung" dataDxfId="23"/>
+    <tableColumn id="3" name="Erwartetes Ergebnis" dataDxfId="22"/>
+    <tableColumn id="4" name="Check"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table367" displayName="Table367" ref="B69:E79" totalsRowShown="0">
+  <autoFilter ref="B69:E79"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Sut" dataDxfId="21"/>
+    <tableColumn id="2" name="Testbedingung" dataDxfId="20"/>
+    <tableColumn id="3" name="Erwartetes Ergebnis" dataDxfId="19"/>
+    <tableColumn id="4" name="Check"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="B83:E99" totalsRowShown="0" headerRowDxfId="15" dataDxfId="6" headerRowBorderDxfId="17" tableBorderDxfId="18" totalsRowBorderDxfId="16">
+  <autoFilter ref="B83:E99"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Sut" dataDxfId="10" totalsRowDxfId="14"/>
+    <tableColumn id="2" name="Testbedingung" dataDxfId="9" totalsRowDxfId="13"/>
+    <tableColumn id="3" name="Erwartetes Ergebnis" dataDxfId="8" totalsRowDxfId="12"/>
+    <tableColumn id="4" name="Check" dataDxfId="7" totalsRowDxfId="11"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table359" displayName="Table359" ref="B103:E114" totalsRowShown="0">
+  <autoFilter ref="B103:E114"/>
+  <tableColumns count="4">
     <tableColumn id="1" name="Sut" dataDxfId="5"/>
     <tableColumn id="2" name="Testbedingung" dataDxfId="4"/>
     <tableColumn id="3" name="Erwartetes Ergebnis" dataDxfId="3"/>
@@ -882,9 +1573,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table36" displayName="Table36" ref="B41:E65" totalsRowShown="0">
-  <autoFilter ref="B41:E65"/>
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table35910" displayName="Table35910" ref="B118:E128" totalsRowShown="0">
+  <autoFilter ref="B118:E128"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Sut" dataDxfId="2"/>
     <tableColumn id="2" name="Testbedingung" dataDxfId="1"/>
@@ -1185,7 +1876,7 @@
   <dimension ref="B2:I38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -2001,10 +2692,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E65"/>
+  <dimension ref="B2:E121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C78" sqref="C78"/>
+    <sheetView tabSelected="1" topLeftCell="A112" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G123" sqref="G123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -2640,7 +3331,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="65" spans="3:5" ht="57.1" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:5" ht="57.1" x14ac:dyDescent="0.25">
       <c r="C65" s="1" t="s">
         <v>178</v>
       </c>
@@ -2648,16 +3339,594 @@
         <v>173</v>
       </c>
       <c r="E65" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B67" s="11" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B69" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E69" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B70" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="E70" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="71" spans="2:5" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="C71" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="E71" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C72" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="E72" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="73" spans="2:5" ht="71.349999999999994" x14ac:dyDescent="0.25">
+      <c r="C73" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="E73" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="74" spans="2:5" ht="71.349999999999994" x14ac:dyDescent="0.25">
+      <c r="C74" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="E74" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="75" spans="2:5" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="B75" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="E75" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="76" spans="2:5" ht="71.349999999999994" x14ac:dyDescent="0.25">
+      <c r="C76" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="E76" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="77" spans="2:5" ht="57.1" x14ac:dyDescent="0.25">
+      <c r="C77" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="E77" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="78" spans="2:5" ht="42.8" x14ac:dyDescent="0.25">
+      <c r="C78" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="79" spans="2:5" ht="42.8" x14ac:dyDescent="0.25">
+      <c r="C79" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="E79" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="81" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B81" s="11" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="83" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B83" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="C83" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="D83" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="E83" s="13" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="84" spans="2:5" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="B84" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="C84" s="9"/>
+      <c r="D84" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="E84" s="9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="85" spans="2:5" ht="57.1" x14ac:dyDescent="0.25">
+      <c r="B85" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="C85" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="D85" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="E85" s="9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="86" spans="2:5" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="B86" s="10" t="s">
+        <v>226</v>
+      </c>
+      <c r="C86" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="D86" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="E86" s="10" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="87" spans="2:5" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="B87" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="C87" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="D87" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="E87" s="9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="88" spans="2:5" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="B88" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="C88" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="D88" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="E88" s="10" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="89" spans="2:5" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="B89" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="C89" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="D89" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="E89" s="9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="90" spans="2:5" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="B90" s="10" t="s">
+        <v>235</v>
+      </c>
+      <c r="C90" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="D90" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="E90" s="10" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="91" spans="2:5" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="B91" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C91" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="92" spans="2:5" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="B92" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C92" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="E92" s="9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="93" spans="2:5" ht="42.8" x14ac:dyDescent="0.25">
+      <c r="B93" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="C93" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="D93" s="14" t="s">
+        <v>241</v>
+      </c>
+      <c r="E93" s="14" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="94" spans="2:5" ht="42.8" x14ac:dyDescent="0.25">
+      <c r="B94" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="C94" s="10" t="s">
+        <v>242</v>
+      </c>
+      <c r="D94" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="E94" s="9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="95" spans="2:5" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="B95" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="C95" s="10" t="s">
+        <v>244</v>
+      </c>
+      <c r="D95" s="9" t="s">
+        <v>245</v>
+      </c>
+      <c r="E95" s="9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="96" spans="2:5" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="B96" s="10" t="s">
+        <v>226</v>
+      </c>
+      <c r="C96" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="D96" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="E96" s="9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="97" spans="2:5" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="B97" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="C97" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="D97" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="E97" s="9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="98" spans="2:5" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="B98" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="C98" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="D98" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="E98" s="9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="99" spans="2:5" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="B99" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="C99" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="D99" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="E99" s="9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="101" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B101" s="8" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="103" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B103" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E103" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="104" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B104" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="E104" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="105" spans="2:5" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="B105" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="E105" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="106" spans="2:5" ht="42.8" x14ac:dyDescent="0.25">
+      <c r="B106" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="E106" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="107" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B107" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="E107" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="108" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B108" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="E108" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="109" spans="2:5" ht="42.8" x14ac:dyDescent="0.25">
+      <c r="B109" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="E109" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="110" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B110" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="E110" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="111" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B111" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="E111" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="112" spans="2:5" ht="71.349999999999994" x14ac:dyDescent="0.25">
+      <c r="D112" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="E112" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="113" spans="2:5" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="B113" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="E113" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="114" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B114" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="E114" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="116" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B116" s="8" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="118" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B118" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E118" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="119" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B119" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="120" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B120" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="D120" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="121" spans="2:5" ht="42.8" x14ac:dyDescent="0.25">
+      <c r="B121" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="E121" t="s">
         <v>109</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="3">
+  <tableParts count="7">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId8"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Updated Layout of TimerWindow
</commit_message>
<xml_diff>
--- a/Bus, Erweiterungen, Tests.xlsx
+++ b/Bus, Erweiterungen, Tests.xlsx
@@ -1049,40 +1049,11 @@
           <bgColor theme="4" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -1145,12 +1116,8 @@
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -1209,11 +1176,46 @@
           <bgColor theme="4" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
         <top/>
         <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -1272,8 +1274,35 @@
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
-        <top/>
-        <bottom/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <right style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -1299,11 +1328,12 @@
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -1329,36 +1359,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </left>
-        <right style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </right>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1548,13 +1548,13 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="B83:E99" totalsRowShown="0" headerRowDxfId="15" dataDxfId="6" headerRowBorderDxfId="17" tableBorderDxfId="18" totalsRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="B83:E99" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17" tableBorderDxfId="15" totalsRowBorderDxfId="14">
   <autoFilter ref="B83:E99"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Sut" dataDxfId="10" totalsRowDxfId="14"/>
-    <tableColumn id="2" name="Testbedingung" dataDxfId="9" totalsRowDxfId="13"/>
-    <tableColumn id="3" name="Erwartetes Ergebnis" dataDxfId="8" totalsRowDxfId="12"/>
-    <tableColumn id="4" name="Check" dataDxfId="7" totalsRowDxfId="11"/>
+    <tableColumn id="1" name="Sut" dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="2" name="Testbedingung" dataDxfId="11" totalsRowDxfId="10"/>
+    <tableColumn id="3" name="Erwartetes Ergebnis" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="4" name="Check" dataDxfId="7" totalsRowDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1876,7 +1876,7 @@
   <dimension ref="B2:I38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -2694,7 +2694,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A109" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="G123" sqref="G123"/>
     </sheetView>
   </sheetViews>

</xml_diff>